<commit_message>
added behav cat to events export
</commit_message>
<xml_diff>
--- a/tests/files/test_export_events_tabular.xlsx
+++ b/tests/files/test_export_events_tabular.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Observation id</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Behavior</t>
+  </si>
+  <si>
+    <t>Behavioral category</t>
   </si>
   <si>
     <t>Comment</t>
@@ -745,206 +748,208 @@
       <c r="H19" t="s">
         <v>26</v>
       </c>
-      <c r="I19" t="s"/>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s"/>
       <c r="H20" t="s"/>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G21" t="s"/>
       <c r="H21" t="s"/>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s"/>
       <c r="H22" t="s"/>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s"/>
       <c r="H23" t="s"/>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s"/>
       <c r="H24" t="s"/>
       <c r="I24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G25" t="s"/>
       <c r="H25" t="s"/>
       <c r="I25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s"/>
       <c r="H26" t="s"/>
       <c r="I26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s"/>
       <c r="H27" t="s"/>
       <c r="I27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>